<commit_message>
Ändrat så att header=None
</commit_message>
<xml_diff>
--- a/KLTelFörbr.xlsx
+++ b/KLTelFörbr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ce47301d0b58e66/Dokument/Energigemenskaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D91855BD-D008-4746-B730-C0A8E0B4D21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D91855BD-D008-4746-B730-C0A8E0B4D21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B6E8324-D70B-4FFB-AB76-5CC00F8DD7BD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C021B68-27CF-4502-B5FD-95EA2B03C870}">
-  <dimension ref="A1:A8759"/>
+  <dimension ref="A1:A8760"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A8740" workbookViewId="0">
+      <selection activeCell="C8758" sqref="C8758"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44194,6 +44194,11 @@
         <v>258.54000000000002</v>
       </c>
     </row>
+    <row r="8760" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8760">
+        <v>258.54000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lagt till nätavgift för  södra och kombo
</commit_message>
<xml_diff>
--- a/KLTelFörbr.xlsx
+++ b/KLTelFörbr.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ce47301d0b58e66/Dokument/Energigemenskaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D91855BD-D008-4746-B730-C0A8E0B4D21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B6E8324-D70B-4FFB-AB76-5CC00F8DD7BD}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{D91855BD-D008-4746-B730-C0A8E0B4D21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CACB9ECB-E162-426B-BE69-BE267B61AA74}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -72,6 +83,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C021B68-27CF-4502-B5FD-95EA2B03C870}">
   <dimension ref="A1:A8760"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8740" workbookViewId="0">
-      <selection activeCell="C8758" sqref="C8758"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>